<commit_message>
fix map and adding quest
</commit_message>
<xml_diff>
--- a/Map Enemy Zone.xlsx
+++ b/Map Enemy Zone.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMESTER _3_INFORMATIKA\Logika Komputasional\temp tubes\Tubes-Logkom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7FEB051-D430-4BB3-811E-D6E344449013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611424C0-6B4A-44F8-9453-F24801294443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="2088" windowWidth="17280" windowHeight="8964" xr2:uid="{C6A6DDC5-96D5-48C8-8302-D31D91D2262D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6A6DDC5-96D5-48C8-8302-D31D91D2262D}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>SLIME</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>LAMIA</t>
+  </si>
+  <si>
+    <t>Quest, Store, and Player Spawn Zone</t>
+  </si>
+  <si>
+    <t>Quest and Store Spawn Zone</t>
   </si>
 </sst>
 </file>
@@ -116,7 +122,7 @@
       <family val="4"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +165,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -285,11 +303,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -299,32 +434,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,20 +464,48 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6743C7B-6DF1-4AE8-A5CB-E2F51D20FEAE}">
   <dimension ref="A1:AO44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +863,7 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
+      <c r="AI1" s="5"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -719,21 +873,21 @@
     </row>
     <row r="2" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -742,43 +896,43 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="6"/>
-      <c r="V2" s="20" t="s">
+      <c r="V2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="18"/>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="18"/>
-      <c r="AN2" s="18"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="15"/>
       <c r="AO2" s="6"/>
     </row>
     <row r="3" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="5"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -787,39 +941,39 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="6"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
-      <c r="AK3" s="18"/>
-      <c r="AL3" s="18"/>
-      <c r="AM3" s="18"/>
-      <c r="AN3" s="18"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="15"/>
+      <c r="AE3" s="15"/>
+      <c r="AF3" s="15"/>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="15"/>
+      <c r="AI3" s="15"/>
+      <c r="AJ3" s="15"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="15"/>
+      <c r="AM3" s="15"/>
+      <c r="AN3" s="15"/>
       <c r="AO3" s="6"/>
     </row>
     <row r="4" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="5"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -828,162 +982,162 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="6"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="21"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="18"/>
-      <c r="AI4" s="18"/>
-      <c r="AJ4" s="18"/>
-      <c r="AK4" s="18"/>
-      <c r="AL4" s="18"/>
-      <c r="AM4" s="18"/>
-      <c r="AN4" s="18"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
+      <c r="AN4" s="15"/>
       <c r="AO4" s="6"/>
     </row>
     <row r="5" spans="1:41" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
       <c r="T5" s="6"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="18"/>
-      <c r="AH5" s="18"/>
-      <c r="AI5" s="18"/>
-      <c r="AJ5" s="18"/>
-      <c r="AK5" s="18"/>
-      <c r="AL5" s="18"/>
-      <c r="AM5" s="18"/>
-      <c r="AN5" s="18"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
       <c r="AO5" s="6"/>
     </row>
     <row r="6" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
       <c r="T6" s="6"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="18"/>
-      <c r="AH6" s="18"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="18"/>
-      <c r="AL6" s="18"/>
-      <c r="AM6" s="18"/>
-      <c r="AN6" s="18"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="15"/>
       <c r="AO6" s="6"/>
     </row>
     <row r="7" spans="1:41" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
       <c r="T7" s="6"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
-      <c r="AC7" s="18"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="18"/>
-      <c r="AH7" s="18"/>
-      <c r="AI7" s="18"/>
-      <c r="AJ7" s="18"/>
-      <c r="AK7" s="18"/>
-      <c r="AL7" s="18"/>
-      <c r="AM7" s="18"/>
-      <c r="AN7" s="18"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="15"/>
+      <c r="AM7" s="15"/>
+      <c r="AN7" s="15"/>
       <c r="AO7" s="6"/>
     </row>
     <row r="8" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
       <c r="T8" s="6"/>
       <c r="V8" s="1"/>
       <c r="W8" s="5"/>
@@ -993,18 +1147,18 @@
       <c r="Y8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="18"/>
-      <c r="AI8" s="18"/>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="15"/>
+      <c r="AJ8" s="15"/>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="15"/>
+      <c r="AN8" s="15"/>
       <c r="AO8" s="6"/>
     </row>
     <row r="9" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1017,12 +1171,12 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
       <c r="T9" s="6"/>
       <c r="V9" s="4"/>
       <c r="W9" s="5" t="s">
@@ -1036,18 +1190,18 @@
       </c>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
-      <c r="AC9" s="18"/>
-      <c r="AD9" s="18"/>
-      <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
-      <c r="AG9" s="18"/>
-      <c r="AH9" s="18"/>
-      <c r="AI9" s="18"/>
-      <c r="AJ9" s="18"/>
-      <c r="AK9" s="18"/>
-      <c r="AL9" s="18"/>
-      <c r="AM9" s="18"/>
-      <c r="AN9" s="18"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="15"/>
+      <c r="AK9" s="15"/>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="15"/>
+      <c r="AN9" s="15"/>
       <c r="AO9" s="6"/>
     </row>
     <row r="10" spans="1:41" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1057,19 +1211,19 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
       <c r="T10" s="6"/>
       <c r="V10" s="7"/>
       <c r="W10" s="5"/>
@@ -1079,18 +1233,18 @@
       <c r="Y10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
-      <c r="AE10" s="18"/>
-      <c r="AF10" s="18"/>
-      <c r="AG10" s="18"/>
-      <c r="AH10" s="18"/>
-      <c r="AI10" s="18"/>
-      <c r="AJ10" s="18"/>
-      <c r="AK10" s="18"/>
-      <c r="AL10" s="18"/>
-      <c r="AM10" s="18"/>
-      <c r="AN10" s="18"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
+      <c r="AI10" s="15"/>
+      <c r="AJ10" s="15"/>
+      <c r="AK10" s="15"/>
+      <c r="AL10" s="15"/>
+      <c r="AM10" s="15"/>
+      <c r="AN10" s="15"/>
       <c r="AO10" s="6"/>
     </row>
     <row r="11" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1100,54 +1254,54 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="26"/>
       <c r="T11" s="6"/>
-      <c r="V11" s="20" t="s">
+      <c r="V11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="18"/>
-      <c r="AG11" s="18"/>
-      <c r="AH11" s="18"/>
-      <c r="AI11" s="18"/>
-      <c r="AJ11" s="18"/>
-      <c r="AK11" s="18"/>
-      <c r="AL11" s="18"/>
-      <c r="AM11" s="18"/>
-      <c r="AN11" s="18"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
+      <c r="AI11" s="15"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="15"/>
+      <c r="AM11" s="15"/>
+      <c r="AN11" s="15"/>
       <c r="AO11" s="6"/>
     </row>
     <row r="12" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1158,149 +1312,149 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="6"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="18"/>
-      <c r="AG12" s="18"/>
-      <c r="AH12" s="18"/>
-      <c r="AI12" s="18"/>
-      <c r="AJ12" s="18"/>
-      <c r="AK12" s="18"/>
-      <c r="AL12" s="18"/>
-      <c r="AM12" s="18"/>
-      <c r="AN12" s="18"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="15"/>
+      <c r="AH12" s="15"/>
+      <c r="AI12" s="15"/>
+      <c r="AJ12" s="15"/>
+      <c r="AK12" s="15"/>
+      <c r="AL12" s="15"/>
+      <c r="AM12" s="15"/>
+      <c r="AN12" s="15"/>
       <c r="AO12" s="6"/>
     </row>
     <row r="13" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="6"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18"/>
-      <c r="AI13" s="18"/>
-      <c r="AJ13" s="18"/>
-      <c r="AK13" s="18"/>
-      <c r="AL13" s="18"/>
-      <c r="AM13" s="18"/>
-      <c r="AN13" s="18"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="15"/>
+      <c r="AL13" s="15"/>
+      <c r="AM13" s="15"/>
+      <c r="AN13" s="15"/>
       <c r="AO13" s="6"/>
     </row>
     <row r="14" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="5"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="6"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="18"/>
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18"/>
+      <c r="Z14" s="18"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="18"/>
-      <c r="AF14" s="18"/>
-      <c r="AG14" s="18"/>
-      <c r="AH14" s="18"/>
-      <c r="AI14" s="18"/>
-      <c r="AJ14" s="18"/>
-      <c r="AK14" s="18"/>
-      <c r="AL14" s="18"/>
-      <c r="AM14" s="18"/>
-      <c r="AN14" s="18"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="15"/>
       <c r="AO14" s="6"/>
     </row>
     <row r="15" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="5"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="6"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
-      <c r="AC15" s="18"/>
-      <c r="AD15" s="18"/>
-      <c r="AE15" s="18"/>
-      <c r="AF15" s="18"/>
-      <c r="AG15" s="18"/>
-      <c r="AH15" s="18"/>
-      <c r="AI15" s="18"/>
-      <c r="AJ15" s="18"/>
-      <c r="AK15" s="18"/>
-      <c r="AL15" s="18"/>
-      <c r="AM15" s="18"/>
-      <c r="AN15" s="18"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="15"/>
+      <c r="AL15" s="15"/>
+      <c r="AM15" s="15"/>
+      <c r="AN15" s="15"/>
       <c r="AO15" s="6"/>
     </row>
     <row r="16" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1309,38 +1463,38 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="6"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="18"/>
-      <c r="AH16" s="18"/>
-      <c r="AI16" s="18"/>
-      <c r="AJ16" s="18"/>
-      <c r="AK16" s="18"/>
-      <c r="AL16" s="18"/>
-      <c r="AM16" s="18"/>
-      <c r="AN16" s="18"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="15"/>
       <c r="AO16" s="6"/>
     </row>
     <row r="17" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1349,16 +1503,16 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
@@ -1369,18 +1523,18 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
-      <c r="AH17" s="18"/>
-      <c r="AI17" s="18"/>
-      <c r="AJ17" s="18"/>
-      <c r="AK17" s="18"/>
-      <c r="AL17" s="18"/>
-      <c r="AM17" s="18"/>
-      <c r="AN17" s="18"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="15"/>
+      <c r="AF17" s="15"/>
+      <c r="AG17" s="15"/>
+      <c r="AH17" s="15"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="15"/>
+      <c r="AK17" s="15"/>
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+      <c r="AN17" s="15"/>
       <c r="AO17" s="6"/>
     </row>
     <row r="18" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1389,16 +1543,16 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="6"/>
@@ -1409,18 +1563,18 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
-      <c r="AJ18" s="18"/>
-      <c r="AK18" s="18"/>
-      <c r="AL18" s="18"/>
-      <c r="AM18" s="18"/>
-      <c r="AN18" s="18"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="15"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="15"/>
+      <c r="AK18" s="15"/>
+      <c r="AL18" s="15"/>
+      <c r="AM18" s="15"/>
+      <c r="AN18" s="15"/>
       <c r="AO18" s="6"/>
     </row>
     <row r="19" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1429,12 +1583,12 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="6"/>
@@ -1445,18 +1599,18 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
-      <c r="AC19" s="18"/>
-      <c r="AD19" s="18"/>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="18"/>
-      <c r="AG19" s="18"/>
-      <c r="AH19" s="18"/>
-      <c r="AI19" s="18"/>
-      <c r="AJ19" s="18"/>
-      <c r="AK19" s="18"/>
-      <c r="AL19" s="18"/>
-      <c r="AM19" s="18"/>
-      <c r="AN19" s="18"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="15"/>
+      <c r="AM19" s="15"/>
+      <c r="AN19" s="15"/>
       <c r="AO19" s="6"/>
     </row>
     <row r="20" spans="1:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1479,7 +1633,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
-      <c r="T20" s="14" t="s">
+      <c r="T20" s="9" t="s">
         <v>2</v>
       </c>
       <c r="V20" s="7"/>
@@ -1489,46 +1643,46 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AF20" s="19"/>
-      <c r="AG20" s="19"/>
-      <c r="AH20" s="19"/>
-      <c r="AI20" s="19"/>
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-      <c r="AL20" s="19"/>
-      <c r="AM20" s="19"/>
-      <c r="AN20" s="19"/>
-      <c r="AO20" s="14" t="s">
+      <c r="AC20" s="16"/>
+      <c r="AD20" s="16"/>
+      <c r="AE20" s="16"/>
+      <c r="AF20" s="16"/>
+      <c r="AG20" s="16"/>
+      <c r="AH20" s="16"/>
+      <c r="AI20" s="16"/>
+      <c r="AJ20" s="16"/>
+      <c r="AK20" s="16"/>
+      <c r="AL20" s="16"/>
+      <c r="AM20" s="16"/>
+      <c r="AN20" s="16"/>
+      <c r="AO20" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="17"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="21"/>
     </row>
     <row r="24" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1545,15 +1699,35 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="23" t="s">
+      <c r="N25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="25"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="11"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="39"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="3"/>
     </row>
     <row r="26" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
@@ -1569,13 +1743,33 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="26"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="13"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="34"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+      <c r="AO26" s="6"/>
     </row>
     <row r="27" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
@@ -1591,13 +1785,35 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="26"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="13"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD27" s="40"/>
+      <c r="AE27" s="40"/>
+      <c r="AF27" s="40"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="34"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="6"/>
     </row>
     <row r="28" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
@@ -1613,13 +1829,33 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="26"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="13"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="40"/>
+      <c r="AD28" s="40"/>
+      <c r="AE28" s="40"/>
+      <c r="AF28" s="40"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="34"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="28"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="6"/>
     </row>
     <row r="29" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
@@ -1635,13 +1871,33 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="24"/>
-      <c r="S29" s="24"/>
-      <c r="T29" s="26"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="13"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="33"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="40"/>
+      <c r="AD29" s="40"/>
+      <c r="AE29" s="40"/>
+      <c r="AF29" s="40"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="34"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="28"/>
+      <c r="AL29" s="28"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="6"/>
     </row>
     <row r="30" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
@@ -1657,16 +1913,36 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="26"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="13"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="34"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="28"/>
+      <c r="AK30" s="28"/>
+      <c r="AL30" s="28"/>
+      <c r="AM30" s="29"/>
+      <c r="AN30" s="5"/>
+      <c r="AO30" s="6"/>
     </row>
     <row r="31" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1679,16 +1955,38 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="26"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="13"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="35"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36"/>
+      <c r="AF31" s="36"/>
+      <c r="AG31" s="36"/>
+      <c r="AH31" s="37"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="28"/>
+      <c r="AL31" s="28"/>
+      <c r="AM31" s="28"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="6"/>
     </row>
     <row r="32" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1701,16 +1999,42 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="26"/>
-    </row>
-    <row r="33" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="13"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="28"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="5"/>
+      <c r="AO32" s="6"/>
+    </row>
+    <row r="33" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1723,16 +2047,46 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="24"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="26"/>
-    </row>
-    <row r="34" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="13"/>
+      <c r="V33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5"/>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="6"/>
+    </row>
+    <row r="34" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1745,16 +2099,42 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="26"/>
-    </row>
-    <row r="35" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="13"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="X34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="5"/>
+      <c r="AC34" s="5"/>
+      <c r="AD34" s="5"/>
+      <c r="AE34" s="5"/>
+      <c r="AF34" s="5"/>
+      <c r="AG34" s="5"/>
+      <c r="AH34" s="5"/>
+      <c r="AI34" s="5"/>
+      <c r="AJ34" s="5"/>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="5"/>
+      <c r="AM34" s="5"/>
+      <c r="AN34" s="5"/>
+      <c r="AO34" s="6"/>
+    </row>
+    <row r="35" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1767,70 +2147,134 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="26"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="13"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y35" s="5"/>
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="5"/>
+      <c r="AC35" s="5"/>
+      <c r="AD35" s="5"/>
+      <c r="AE35" s="5"/>
+      <c r="AF35" s="27"/>
+      <c r="AG35" s="5"/>
+      <c r="AH35" s="5"/>
+      <c r="AI35" s="5"/>
+      <c r="AJ35" s="5"/>
+      <c r="AK35" s="5"/>
+      <c r="AL35" s="5"/>
+      <c r="AM35" s="5"/>
+      <c r="AN35" s="5"/>
+      <c r="AO35" s="6"/>
+    </row>
+    <row r="36" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="26"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="13"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="5"/>
+      <c r="AC36" s="5"/>
+      <c r="AD36" s="5"/>
+      <c r="AE36" s="5"/>
+      <c r="AF36" s="27"/>
+      <c r="AG36" s="27"/>
+      <c r="AH36" s="27"/>
+      <c r="AI36" s="5"/>
+      <c r="AJ36" s="30"/>
+      <c r="AK36" s="31"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="31"/>
+      <c r="AN36" s="32"/>
+      <c r="AO36" s="6"/>
+    </row>
+    <row r="37" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="24"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="26"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="13"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="30"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+      <c r="AB37" s="31"/>
+      <c r="AC37" s="32"/>
+      <c r="AD37" s="5"/>
+      <c r="AE37" s="5"/>
+      <c r="AF37" s="27"/>
+      <c r="AG37" s="27"/>
+      <c r="AH37" s="27"/>
+      <c r="AI37" s="5"/>
+      <c r="AJ37" s="33"/>
+      <c r="AK37" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL37" s="41"/>
+      <c r="AM37" s="41"/>
+      <c r="AN37" s="34"/>
+      <c r="AO37" s="6"/>
+    </row>
+    <row r="38" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -1842,17 +2286,37 @@
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
       <c r="T38" s="6"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V38" s="4"/>
+      <c r="W38" s="33"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="5"/>
+      <c r="AC38" s="34"/>
+      <c r="AD38" s="5"/>
+      <c r="AE38" s="27"/>
+      <c r="AF38" s="27"/>
+      <c r="AG38" s="27"/>
+      <c r="AH38" s="27"/>
+      <c r="AI38" s="5"/>
+      <c r="AJ38" s="33"/>
+      <c r="AK38" s="41"/>
+      <c r="AL38" s="41"/>
+      <c r="AM38" s="41"/>
+      <c r="AN38" s="34"/>
+      <c r="AO38" s="6"/>
+    </row>
+    <row r="39" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -1864,17 +2328,39 @@
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
       <c r="T39" s="6"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V39" s="4"/>
+      <c r="W39" s="33"/>
+      <c r="X39" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="40"/>
+      <c r="AA39" s="40"/>
+      <c r="AB39" s="40"/>
+      <c r="AC39" s="34"/>
+      <c r="AD39" s="5"/>
+      <c r="AE39" s="27"/>
+      <c r="AF39" s="27"/>
+      <c r="AG39" s="27"/>
+      <c r="AH39" s="27"/>
+      <c r="AI39" s="5"/>
+      <c r="AJ39" s="33"/>
+      <c r="AK39" s="41"/>
+      <c r="AL39" s="41"/>
+      <c r="AM39" s="41"/>
+      <c r="AN39" s="34"/>
+      <c r="AO39" s="6"/>
+    </row>
+    <row r="40" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -1886,17 +2372,37 @@
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="6"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V40" s="4"/>
+      <c r="W40" s="33"/>
+      <c r="X40" s="40"/>
+      <c r="Y40" s="40"/>
+      <c r="Z40" s="40"/>
+      <c r="AA40" s="40"/>
+      <c r="AB40" s="40"/>
+      <c r="AC40" s="34"/>
+      <c r="AD40" s="5"/>
+      <c r="AE40" s="27"/>
+      <c r="AF40" s="27"/>
+      <c r="AG40" s="27"/>
+      <c r="AH40" s="27"/>
+      <c r="AI40" s="5"/>
+      <c r="AJ40" s="33"/>
+      <c r="AK40" s="41"/>
+      <c r="AL40" s="41"/>
+      <c r="AM40" s="41"/>
+      <c r="AN40" s="34"/>
+      <c r="AO40" s="6"/>
+    </row>
+    <row r="41" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -1908,21 +2414,37 @@
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
       <c r="T41" s="6"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V41" s="4"/>
+      <c r="W41" s="33"/>
+      <c r="X41" s="40"/>
+      <c r="Y41" s="40"/>
+      <c r="Z41" s="40"/>
+      <c r="AA41" s="40"/>
+      <c r="AB41" s="40"/>
+      <c r="AC41" s="34"/>
+      <c r="AD41" s="5"/>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="27"/>
+      <c r="AG41" s="27"/>
+      <c r="AH41" s="5"/>
+      <c r="AI41" s="5"/>
+      <c r="AJ41" s="33"/>
+      <c r="AK41" s="41"/>
+      <c r="AL41" s="41"/>
+      <c r="AM41" s="41"/>
+      <c r="AN41" s="34"/>
+      <c r="AO41" s="6"/>
+    </row>
+    <row r="42" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
@@ -1930,8 +2452,28 @@
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
       <c r="T42" s="6"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V42" s="4"/>
+      <c r="W42" s="33"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="5"/>
+      <c r="AC42" s="34"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="5"/>
+      <c r="AF42" s="5"/>
+      <c r="AG42" s="5"/>
+      <c r="AH42" s="5"/>
+      <c r="AI42" s="5"/>
+      <c r="AJ42" s="35"/>
+      <c r="AK42" s="36"/>
+      <c r="AL42" s="36"/>
+      <c r="AM42" s="36"/>
+      <c r="AN42" s="37"/>
+      <c r="AO42" s="6"/>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1941,10 +2483,6 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
       <c r="N43" s="5"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
@@ -1952,8 +2490,28 @@
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
       <c r="T43" s="6"/>
-    </row>
-    <row r="44" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V43" s="4"/>
+      <c r="W43" s="35"/>
+      <c r="X43" s="36"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="36"/>
+      <c r="AA43" s="36"/>
+      <c r="AB43" s="36"/>
+      <c r="AC43" s="37"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="5"/>
+      <c r="AH43" s="5"/>
+      <c r="AI43" s="5"/>
+      <c r="AJ43" s="5"/>
+      <c r="AK43" s="5"/>
+      <c r="AL43" s="5"/>
+      <c r="AM43" s="5"/>
+      <c r="AN43" s="5"/>
+      <c r="AO43" s="6"/>
+    </row>
+    <row r="44" spans="1:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -1973,12 +2531,36 @@
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
-      <c r="T44" s="14" t="s">
+      <c r="T44" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="V44" s="7"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+      <c r="Z44" s="8"/>
+      <c r="AA44" s="8"/>
+      <c r="AB44" s="8"/>
+      <c r="AC44" s="8"/>
+      <c r="AD44" s="8"/>
+      <c r="AE44" s="8"/>
+      <c r="AF44" s="8"/>
+      <c r="AG44" s="8"/>
+      <c r="AH44" s="8"/>
+      <c r="AI44" s="8"/>
+      <c r="AJ44" s="8"/>
+      <c r="AK44" s="8"/>
+      <c r="AL44" s="8"/>
+      <c r="AM44" s="8"/>
+      <c r="AN44" s="8"/>
+      <c r="AO44" s="9" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="X39:AB41"/>
+    <mergeCell ref="AK37:AM41"/>
     <mergeCell ref="N25:T37"/>
     <mergeCell ref="E36:I42"/>
     <mergeCell ref="AC2:AN20"/>
@@ -1991,6 +2573,7 @@
     <mergeCell ref="B2:G8"/>
     <mergeCell ref="N5:S11"/>
     <mergeCell ref="L13:Q19"/>
+    <mergeCell ref="AC27:AF29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
break after enemy defeated
</commit_message>
<xml_diff>
--- a/Map Enemy Zone.xlsx
+++ b/Map Enemy Zone.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMESTER _3_INFORMATIKA\Logika Komputasional\temp tubes\Tubes-Logkom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITB\Semester 3\Logkom\Tubes-Logkom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611424C0-6B4A-44F8-9453-F24801294443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38145712-0A1B-447F-8B40-8588BE07C2AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6A6DDC5-96D5-48C8-8302-D31D91D2262D}"/>
   </bookViews>
@@ -60,10 +60,10 @@
     <t>LAMIA</t>
   </si>
   <si>
-    <t>Quest, Store, and Player Spawn Zone</t>
+    <t>Quest and Store Spawn Zone</t>
   </si>
   <si>
-    <t>Quest and Store Spawn Zone</t>
+    <t>Player Spawn Zone</t>
   </si>
 </sst>
 </file>
@@ -437,6 +437,25 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,25 +507,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +525,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6743C7B-6DF1-4AE8-A5CB-E2F51D20FEAE}">
   <dimension ref="A1:AO44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="W22" workbookViewId="0">
+      <selection activeCell="AD35" sqref="AD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,21 +873,21 @@
     </row>
     <row r="2" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -896,43 +896,43 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="6"/>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
-      <c r="AC2" s="15" t="s">
+      <c r="AC2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
       <c r="AO2" s="6"/>
     </row>
     <row r="3" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="5"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -941,39 +941,39 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="6"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="30"/>
+      <c r="AE3" s="30"/>
+      <c r="AF3" s="30"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="30"/>
+      <c r="AJ3" s="30"/>
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="30"/>
+      <c r="AM3" s="30"/>
+      <c r="AN3" s="30"/>
       <c r="AO3" s="6"/>
     </row>
     <row r="4" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="5"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -982,162 +982,162 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="6"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="30"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="30"/>
       <c r="AO4" s="6"/>
     </row>
     <row r="5" spans="1:41" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="5"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
       <c r="T5" s="6"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
+      <c r="AC5" s="30"/>
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="30"/>
+      <c r="AJ5" s="30"/>
+      <c r="AK5" s="30"/>
+      <c r="AL5" s="30"/>
+      <c r="AM5" s="30"/>
+      <c r="AN5" s="30"/>
       <c r="AO5" s="6"/>
     </row>
     <row r="6" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
       <c r="T6" s="6"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
+      <c r="AC6" s="30"/>
+      <c r="AD6" s="30"/>
+      <c r="AE6" s="30"/>
+      <c r="AF6" s="30"/>
+      <c r="AG6" s="30"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="30"/>
+      <c r="AK6" s="30"/>
+      <c r="AL6" s="30"/>
+      <c r="AM6" s="30"/>
+      <c r="AN6" s="30"/>
       <c r="AO6" s="6"/>
     </row>
     <row r="7" spans="1:41" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
       <c r="H7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
       <c r="T7" s="6"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
-      <c r="AG7" s="15"/>
-      <c r="AH7" s="15"/>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="15"/>
-      <c r="AK7" s="15"/>
-      <c r="AL7" s="15"/>
-      <c r="AM7" s="15"/>
-      <c r="AN7" s="15"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
+      <c r="AH7" s="30"/>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="30"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="30"/>
+      <c r="AM7" s="30"/>
+      <c r="AN7" s="30"/>
       <c r="AO7" s="6"/>
     </row>
     <row r="8" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
       <c r="T8" s="6"/>
       <c r="V8" s="1"/>
       <c r="W8" s="5"/>
@@ -1147,18 +1147,18 @@
       <c r="Y8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15"/>
-      <c r="AI8" s="15"/>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="15"/>
-      <c r="AL8" s="15"/>
-      <c r="AM8" s="15"/>
-      <c r="AN8" s="15"/>
+      <c r="AC8" s="30"/>
+      <c r="AD8" s="30"/>
+      <c r="AE8" s="30"/>
+      <c r="AF8" s="30"/>
+      <c r="AG8" s="30"/>
+      <c r="AH8" s="30"/>
+      <c r="AI8" s="30"/>
+      <c r="AJ8" s="30"/>
+      <c r="AK8" s="30"/>
+      <c r="AL8" s="30"/>
+      <c r="AM8" s="30"/>
+      <c r="AN8" s="30"/>
       <c r="AO8" s="6"/>
     </row>
     <row r="9" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1171,12 +1171,12 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
       <c r="T9" s="6"/>
       <c r="V9" s="4"/>
       <c r="W9" s="5" t="s">
@@ -1190,18 +1190,18 @@
       </c>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-      <c r="AE9" s="15"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="15"/>
-      <c r="AH9" s="15"/>
-      <c r="AI9" s="15"/>
-      <c r="AJ9" s="15"/>
-      <c r="AK9" s="15"/>
-      <c r="AL9" s="15"/>
-      <c r="AM9" s="15"/>
-      <c r="AN9" s="15"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="30"/>
+      <c r="AE9" s="30"/>
+      <c r="AF9" s="30"/>
+      <c r="AG9" s="30"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="30"/>
+      <c r="AJ9" s="30"/>
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="30"/>
+      <c r="AM9" s="30"/>
+      <c r="AN9" s="30"/>
       <c r="AO9" s="6"/>
     </row>
     <row r="10" spans="1:41" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1211,19 +1211,19 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
       <c r="T10" s="6"/>
       <c r="V10" s="7"/>
       <c r="W10" s="5"/>
@@ -1233,18 +1233,18 @@
       <c r="Y10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
-      <c r="AN10" s="15"/>
+      <c r="AC10" s="30"/>
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="30"/>
+      <c r="AF10" s="30"/>
+      <c r="AG10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AI10" s="30"/>
+      <c r="AJ10" s="30"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="30"/>
+      <c r="AM10" s="30"/>
+      <c r="AN10" s="30"/>
       <c r="AO10" s="6"/>
     </row>
     <row r="11" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1254,54 +1254,54 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
       <c r="M11" s="5"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
-      <c r="S11" s="26"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
       <c r="T11" s="6"/>
-      <c r="V11" s="17" t="s">
+      <c r="V11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="15"/>
-      <c r="AG11" s="15"/>
-      <c r="AH11" s="15"/>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="15"/>
-      <c r="AK11" s="15"/>
-      <c r="AL11" s="15"/>
-      <c r="AM11" s="15"/>
-      <c r="AN11" s="15"/>
+      <c r="AC11" s="30"/>
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="30"/>
+      <c r="AF11" s="30"/>
+      <c r="AG11" s="30"/>
+      <c r="AH11" s="30"/>
+      <c r="AI11" s="30"/>
+      <c r="AJ11" s="30"/>
+      <c r="AK11" s="30"/>
+      <c r="AL11" s="30"/>
+      <c r="AM11" s="30"/>
+      <c r="AN11" s="30"/>
       <c r="AO11" s="6"/>
     </row>
     <row r="12" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -1312,149 +1312,149 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="6"/>
-      <c r="V12" s="17"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
+      <c r="Z12" s="33"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="15"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="15"/>
-      <c r="AL12" s="15"/>
-      <c r="AM12" s="15"/>
-      <c r="AN12" s="15"/>
+      <c r="AC12" s="30"/>
+      <c r="AD12" s="30"/>
+      <c r="AE12" s="30"/>
+      <c r="AF12" s="30"/>
+      <c r="AG12" s="30"/>
+      <c r="AH12" s="30"/>
+      <c r="AI12" s="30"/>
+      <c r="AJ12" s="30"/>
+      <c r="AK12" s="30"/>
+      <c r="AL12" s="30"/>
+      <c r="AM12" s="30"/>
+      <c r="AN12" s="30"/>
       <c r="AO12" s="6"/>
     </row>
     <row r="13" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="6"/>
-      <c r="V13" s="17"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
+      <c r="V13" s="32"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
+      <c r="Z13" s="33"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="15"/>
-      <c r="AG13" s="15"/>
-      <c r="AH13" s="15"/>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="15"/>
-      <c r="AK13" s="15"/>
-      <c r="AL13" s="15"/>
-      <c r="AM13" s="15"/>
-      <c r="AN13" s="15"/>
+      <c r="AC13" s="30"/>
+      <c r="AD13" s="30"/>
+      <c r="AE13" s="30"/>
+      <c r="AF13" s="30"/>
+      <c r="AG13" s="30"/>
+      <c r="AH13" s="30"/>
+      <c r="AI13" s="30"/>
+      <c r="AJ13" s="30"/>
+      <c r="AK13" s="30"/>
+      <c r="AL13" s="30"/>
+      <c r="AM13" s="30"/>
+      <c r="AN13" s="30"/>
       <c r="AO13" s="6"/>
     </row>
     <row r="14" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="5"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="6"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-      <c r="AG14" s="15"/>
-      <c r="AH14" s="15"/>
-      <c r="AI14" s="15"/>
-      <c r="AJ14" s="15"/>
-      <c r="AK14" s="15"/>
-      <c r="AL14" s="15"/>
-      <c r="AM14" s="15"/>
-      <c r="AN14" s="15"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AI14" s="30"/>
+      <c r="AJ14" s="30"/>
+      <c r="AK14" s="30"/>
+      <c r="AL14" s="30"/>
+      <c r="AM14" s="30"/>
+      <c r="AN14" s="30"/>
       <c r="AO14" s="6"/>
     </row>
     <row r="15" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="5"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="26"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="6"/>
-      <c r="V15" s="17"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="33"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
+      <c r="Z15" s="33"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
-      <c r="AG15" s="15"/>
-      <c r="AH15" s="15"/>
-      <c r="AI15" s="15"/>
-      <c r="AJ15" s="15"/>
-      <c r="AK15" s="15"/>
-      <c r="AL15" s="15"/>
-      <c r="AM15" s="15"/>
-      <c r="AN15" s="15"/>
+      <c r="AC15" s="30"/>
+      <c r="AD15" s="30"/>
+      <c r="AE15" s="30"/>
+      <c r="AF15" s="30"/>
+      <c r="AG15" s="30"/>
+      <c r="AH15" s="30"/>
+      <c r="AI15" s="30"/>
+      <c r="AJ15" s="30"/>
+      <c r="AK15" s="30"/>
+      <c r="AL15" s="30"/>
+      <c r="AM15" s="30"/>
+      <c r="AN15" s="30"/>
       <c r="AO15" s="6"/>
     </row>
     <row r="16" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1463,38 +1463,38 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="6"/>
-      <c r="V16" s="17"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="33"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
-      <c r="AC16" s="15"/>
-      <c r="AD16" s="15"/>
-      <c r="AE16" s="15"/>
-      <c r="AF16" s="15"/>
-      <c r="AG16" s="15"/>
-      <c r="AH16" s="15"/>
-      <c r="AI16" s="15"/>
-      <c r="AJ16" s="15"/>
-      <c r="AK16" s="15"/>
-      <c r="AL16" s="15"/>
-      <c r="AM16" s="15"/>
-      <c r="AN16" s="15"/>
+      <c r="AC16" s="30"/>
+      <c r="AD16" s="30"/>
+      <c r="AE16" s="30"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="30"/>
+      <c r="AI16" s="30"/>
+      <c r="AJ16" s="30"/>
+      <c r="AK16" s="30"/>
+      <c r="AL16" s="30"/>
+      <c r="AM16" s="30"/>
+      <c r="AN16" s="30"/>
       <c r="AO16" s="6"/>
     </row>
     <row r="17" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1503,16 +1503,16 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
@@ -1523,18 +1523,18 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
-      <c r="AC17" s="15"/>
-      <c r="AD17" s="15"/>
-      <c r="AE17" s="15"/>
-      <c r="AF17" s="15"/>
-      <c r="AG17" s="15"/>
-      <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="15"/>
-      <c r="AK17" s="15"/>
-      <c r="AL17" s="15"/>
-      <c r="AM17" s="15"/>
-      <c r="AN17" s="15"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="30"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="30"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30"/>
       <c r="AO17" s="6"/>
     </row>
     <row r="18" spans="1:41" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1543,16 +1543,16 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="6"/>
@@ -1563,18 +1563,18 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-      <c r="AG18" s="15"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
-      <c r="AM18" s="15"/>
-      <c r="AN18" s="15"/>
+      <c r="AC18" s="30"/>
+      <c r="AD18" s="30"/>
+      <c r="AE18" s="30"/>
+      <c r="AF18" s="30"/>
+      <c r="AG18" s="30"/>
+      <c r="AH18" s="30"/>
+      <c r="AI18" s="30"/>
+      <c r="AJ18" s="30"/>
+      <c r="AK18" s="30"/>
+      <c r="AL18" s="30"/>
+      <c r="AM18" s="30"/>
+      <c r="AN18" s="30"/>
       <c r="AO18" s="6"/>
     </row>
     <row r="19" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1583,12 +1583,12 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="6"/>
@@ -1599,18 +1599,18 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="15"/>
-      <c r="AG19" s="15"/>
-      <c r="AH19" s="15"/>
-      <c r="AI19" s="15"/>
-      <c r="AJ19" s="15"/>
-      <c r="AK19" s="15"/>
-      <c r="AL19" s="15"/>
-      <c r="AM19" s="15"/>
-      <c r="AN19" s="15"/>
+      <c r="AC19" s="30"/>
+      <c r="AD19" s="30"/>
+      <c r="AE19" s="30"/>
+      <c r="AF19" s="30"/>
+      <c r="AG19" s="30"/>
+      <c r="AH19" s="30"/>
+      <c r="AI19" s="30"/>
+      <c r="AJ19" s="30"/>
+      <c r="AK19" s="30"/>
+      <c r="AL19" s="30"/>
+      <c r="AM19" s="30"/>
+      <c r="AN19" s="30"/>
       <c r="AO19" s="6"/>
     </row>
     <row r="20" spans="1:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1643,46 +1643,46 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
-      <c r="AC20" s="16"/>
-      <c r="AD20" s="16"/>
-      <c r="AE20" s="16"/>
-      <c r="AF20" s="16"/>
-      <c r="AG20" s="16"/>
-      <c r="AH20" s="16"/>
-      <c r="AI20" s="16"/>
-      <c r="AJ20" s="16"/>
-      <c r="AK20" s="16"/>
-      <c r="AL20" s="16"/>
-      <c r="AM20" s="16"/>
-      <c r="AN20" s="16"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="31"/>
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="31"/>
+      <c r="AI20" s="31"/>
+      <c r="AJ20" s="31"/>
+      <c r="AK20" s="31"/>
+      <c r="AL20" s="31"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="31"/>
       <c r="AO20" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="21"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="36"/>
     </row>
     <row r="24" spans="1:41" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1699,28 +1699,28 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="10" t="s">
+      <c r="N25" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="11"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="26"/>
       <c r="V25" s="1"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
-      <c r="AA25" s="38"/>
+      <c r="AA25" s="21"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
       <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
-      <c r="AH25" s="39"/>
+      <c r="AH25" s="22"/>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
       <c r="AK25" s="2"/>
@@ -1743,26 +1743,26 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="12"/>
-      <c r="T26" s="13"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="28"/>
       <c r="V26" s="4"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
-      <c r="AA26" s="33"/>
+      <c r="AA26" s="16"/>
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
       <c r="AE26" s="5"/>
       <c r="AF26" s="5"/>
       <c r="AG26" s="5"/>
-      <c r="AH26" s="34"/>
+      <c r="AH26" s="17"/>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
       <c r="AK26" s="5"/>
@@ -1785,28 +1785,28 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="13"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="28"/>
       <c r="V27" s="4"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
-      <c r="AA27" s="33"/>
+      <c r="AA27" s="16"/>
       <c r="AB27" s="5"/>
-      <c r="AC27" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD27" s="40"/>
-      <c r="AE27" s="40"/>
-      <c r="AF27" s="40"/>
+      <c r="AC27" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD27" s="23"/>
+      <c r="AE27" s="23"/>
+      <c r="AF27" s="23"/>
       <c r="AG27" s="5"/>
-      <c r="AH27" s="34"/>
+      <c r="AH27" s="17"/>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
@@ -1829,30 +1829,30 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="12"/>
-      <c r="T28" s="13"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="28"/>
       <c r="V28" s="4"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
-      <c r="AA28" s="33"/>
+      <c r="AA28" s="16"/>
       <c r="AB28" s="5"/>
-      <c r="AC28" s="40"/>
-      <c r="AD28" s="40"/>
-      <c r="AE28" s="40"/>
-      <c r="AF28" s="40"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
       <c r="AG28" s="5"/>
-      <c r="AH28" s="34"/>
+      <c r="AH28" s="17"/>
       <c r="AI28" s="5"/>
       <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
-      <c r="AL28" s="28"/>
+      <c r="AL28" s="11"/>
       <c r="AM28" s="5"/>
       <c r="AN28" s="5"/>
       <c r="AO28" s="6"/>
@@ -1871,30 +1871,30 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="13"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="28"/>
       <c r="V29" s="4"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
-      <c r="AA29" s="33"/>
+      <c r="AA29" s="16"/>
       <c r="AB29" s="5"/>
-      <c r="AC29" s="40"/>
-      <c r="AD29" s="40"/>
-      <c r="AE29" s="40"/>
-      <c r="AF29" s="40"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="23"/>
+      <c r="AE29" s="23"/>
+      <c r="AF29" s="23"/>
       <c r="AG29" s="5"/>
-      <c r="AH29" s="34"/>
+      <c r="AH29" s="17"/>
       <c r="AI29" s="5"/>
       <c r="AJ29" s="5"/>
-      <c r="AK29" s="28"/>
-      <c r="AL29" s="28"/>
+      <c r="AK29" s="11"/>
+      <c r="AL29" s="11"/>
       <c r="AM29" s="5"/>
       <c r="AN29" s="5"/>
       <c r="AO29" s="6"/>
@@ -1913,31 +1913,31 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="12"/>
-      <c r="R30" s="12"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="13"/>
+      <c r="N30" s="27"/>
+      <c r="O30" s="27"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="27"/>
+      <c r="R30" s="27"/>
+      <c r="S30" s="27"/>
+      <c r="T30" s="28"/>
       <c r="V30" s="4"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
-      <c r="AA30" s="33"/>
+      <c r="AA30" s="16"/>
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
       <c r="AD30" s="5"/>
       <c r="AE30" s="5"/>
       <c r="AF30" s="5"/>
       <c r="AG30" s="5"/>
-      <c r="AH30" s="34"/>
+      <c r="AH30" s="17"/>
       <c r="AI30" s="5"/>
-      <c r="AJ30" s="28"/>
-      <c r="AK30" s="28"/>
-      <c r="AL30" s="28"/>
-      <c r="AM30" s="29"/>
+      <c r="AJ30" s="11"/>
+      <c r="AK30" s="11"/>
+      <c r="AL30" s="11"/>
+      <c r="AM30" s="12"/>
       <c r="AN30" s="5"/>
       <c r="AO30" s="6"/>
     </row>
@@ -1955,13 +1955,13 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-      <c r="S31" s="12"/>
-      <c r="T31" s="13"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="28"/>
       <c r="V31" s="4"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5" t="s">
@@ -1969,19 +1969,19 @@
       </c>
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
-      <c r="AA31" s="35"/>
-      <c r="AB31" s="36"/>
-      <c r="AC31" s="36"/>
-      <c r="AD31" s="36"/>
-      <c r="AE31" s="36"/>
-      <c r="AF31" s="36"/>
-      <c r="AG31" s="36"/>
-      <c r="AH31" s="37"/>
+      <c r="AA31" s="18"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="20"/>
       <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
-      <c r="AK31" s="28"/>
-      <c r="AL31" s="28"/>
-      <c r="AM31" s="28"/>
+      <c r="AK31" s="11"/>
+      <c r="AL31" s="11"/>
+      <c r="AM31" s="11"/>
       <c r="AN31" s="5"/>
       <c r="AO31" s="6"/>
     </row>
@@ -1999,13 +1999,13 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
-      <c r="S32" s="12"/>
-      <c r="T32" s="13"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="28"/>
       <c r="V32" s="4"/>
       <c r="W32" s="5" t="s">
         <v>5</v>
@@ -2028,7 +2028,7 @@
       <c r="AI32" s="5"/>
       <c r="AJ32" s="5"/>
       <c r="AK32" s="5"/>
-      <c r="AL32" s="28"/>
+      <c r="AL32" s="11"/>
       <c r="AM32" s="5"/>
       <c r="AN32" s="5"/>
       <c r="AO32" s="6"/>
@@ -2047,13 +2047,13 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="12"/>
-      <c r="S33" s="12"/>
-      <c r="T33" s="13"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
+      <c r="P33" s="27"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="28"/>
       <c r="V33" s="4" t="s">
         <v>5</v>
       </c>
@@ -2099,13 +2099,13 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="12"/>
-      <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
-      <c r="T34" s="13"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="28"/>
       <c r="V34" s="4"/>
       <c r="W34" s="5" t="s">
         <v>5</v>
@@ -2147,13 +2147,13 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="12"/>
-      <c r="R35" s="12"/>
-      <c r="S35" s="12"/>
-      <c r="T35" s="13"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
+      <c r="P35" s="27"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="27"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="28"/>
       <c r="V35" s="4"/>
       <c r="W35" s="5"/>
       <c r="X35" s="5" t="s">
@@ -2166,7 +2166,7 @@
       <c r="AC35" s="5"/>
       <c r="AD35" s="5"/>
       <c r="AE35" s="5"/>
-      <c r="AF35" s="27"/>
+      <c r="AF35" s="10"/>
       <c r="AG35" s="5"/>
       <c r="AH35" s="5"/>
       <c r="AI35" s="5"/>
@@ -2182,24 +2182,24 @@
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="12"/>
-      <c r="S36" s="12"/>
-      <c r="T36" s="13"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="28"/>
       <c r="V36" s="4"/>
       <c r="W36" s="5"/>
       <c r="X36" s="5"/>
@@ -2210,15 +2210,15 @@
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
       <c r="AE36" s="5"/>
-      <c r="AF36" s="27"/>
-      <c r="AG36" s="27"/>
-      <c r="AH36" s="27"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
+      <c r="AH36" s="10"/>
       <c r="AI36" s="5"/>
-      <c r="AJ36" s="30"/>
-      <c r="AK36" s="31"/>
-      <c r="AL36" s="31"/>
-      <c r="AM36" s="31"/>
-      <c r="AN36" s="32"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="14"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="14"/>
+      <c r="AN36" s="15"/>
       <c r="AO36" s="6"/>
     </row>
     <row r="37" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2226,43 +2226,43 @@
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="13"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="27"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="28"/>
       <c r="V37" s="4"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="31"/>
-      <c r="Y37" s="31"/>
-      <c r="Z37" s="31"/>
-      <c r="AA37" s="31"/>
-      <c r="AB37" s="31"/>
-      <c r="AC37" s="32"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="15"/>
       <c r="AD37" s="5"/>
       <c r="AE37" s="5"/>
-      <c r="AF37" s="27"/>
-      <c r="AG37" s="27"/>
-      <c r="AH37" s="27"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+      <c r="AH37" s="10"/>
       <c r="AI37" s="5"/>
-      <c r="AJ37" s="33"/>
-      <c r="AK37" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL37" s="41"/>
-      <c r="AM37" s="41"/>
-      <c r="AN37" s="34"/>
+      <c r="AJ37" s="16"/>
+      <c r="AK37" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL37" s="24"/>
+      <c r="AM37" s="24"/>
+      <c r="AN37" s="17"/>
       <c r="AO37" s="6"/>
     </row>
     <row r="38" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2270,11 +2270,11 @@
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -2287,24 +2287,24 @@
       <c r="S38" s="5"/>
       <c r="T38" s="6"/>
       <c r="V38" s="4"/>
-      <c r="W38" s="33"/>
+      <c r="W38" s="16"/>
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
       <c r="AB38" s="5"/>
-      <c r="AC38" s="34"/>
+      <c r="AC38" s="17"/>
       <c r="AD38" s="5"/>
-      <c r="AE38" s="27"/>
-      <c r="AF38" s="27"/>
-      <c r="AG38" s="27"/>
-      <c r="AH38" s="27"/>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="10"/>
       <c r="AI38" s="5"/>
-      <c r="AJ38" s="33"/>
-      <c r="AK38" s="41"/>
-      <c r="AL38" s="41"/>
-      <c r="AM38" s="41"/>
-      <c r="AN38" s="34"/>
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="24"/>
+      <c r="AL38" s="24"/>
+      <c r="AM38" s="24"/>
+      <c r="AN38" s="17"/>
       <c r="AO38" s="6"/>
     </row>
     <row r="39" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2312,11 +2312,11 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -2329,26 +2329,26 @@
       <c r="S39" s="5"/>
       <c r="T39" s="6"/>
       <c r="V39" s="4"/>
-      <c r="W39" s="33"/>
-      <c r="X39" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y39" s="40"/>
-      <c r="Z39" s="40"/>
-      <c r="AA39" s="40"/>
-      <c r="AB39" s="40"/>
-      <c r="AC39" s="34"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="23"/>
+      <c r="AA39" s="23"/>
+      <c r="AB39" s="23"/>
+      <c r="AC39" s="17"/>
       <c r="AD39" s="5"/>
-      <c r="AE39" s="27"/>
-      <c r="AF39" s="27"/>
-      <c r="AG39" s="27"/>
-      <c r="AH39" s="27"/>
+      <c r="AE39" s="10"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="10"/>
+      <c r="AH39" s="10"/>
       <c r="AI39" s="5"/>
-      <c r="AJ39" s="33"/>
-      <c r="AK39" s="41"/>
-      <c r="AL39" s="41"/>
-      <c r="AM39" s="41"/>
-      <c r="AN39" s="34"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="24"/>
+      <c r="AL39" s="24"/>
+      <c r="AM39" s="24"/>
+      <c r="AN39" s="17"/>
       <c r="AO39" s="6"/>
     </row>
     <row r="40" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2356,11 +2356,11 @@
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -2373,24 +2373,24 @@
       <c r="S40" s="5"/>
       <c r="T40" s="6"/>
       <c r="V40" s="4"/>
-      <c r="W40" s="33"/>
-      <c r="X40" s="40"/>
-      <c r="Y40" s="40"/>
-      <c r="Z40" s="40"/>
-      <c r="AA40" s="40"/>
-      <c r="AB40" s="40"/>
-      <c r="AC40" s="34"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
+      <c r="AA40" s="23"/>
+      <c r="AB40" s="23"/>
+      <c r="AC40" s="17"/>
       <c r="AD40" s="5"/>
-      <c r="AE40" s="27"/>
-      <c r="AF40" s="27"/>
-      <c r="AG40" s="27"/>
-      <c r="AH40" s="27"/>
+      <c r="AE40" s="10"/>
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="10"/>
+      <c r="AH40" s="10"/>
       <c r="AI40" s="5"/>
-      <c r="AJ40" s="33"/>
-      <c r="AK40" s="41"/>
-      <c r="AL40" s="41"/>
-      <c r="AM40" s="41"/>
-      <c r="AN40" s="34"/>
+      <c r="AJ40" s="16"/>
+      <c r="AK40" s="24"/>
+      <c r="AL40" s="24"/>
+      <c r="AM40" s="24"/>
+      <c r="AN40" s="17"/>
       <c r="AO40" s="6"/>
     </row>
     <row r="41" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2398,11 +2398,11 @@
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -2415,24 +2415,24 @@
       <c r="S41" s="5"/>
       <c r="T41" s="6"/>
       <c r="V41" s="4"/>
-      <c r="W41" s="33"/>
-      <c r="X41" s="40"/>
-      <c r="Y41" s="40"/>
-      <c r="Z41" s="40"/>
-      <c r="AA41" s="40"/>
-      <c r="AB41" s="40"/>
-      <c r="AC41" s="34"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
+      <c r="Z41" s="23"/>
+      <c r="AA41" s="23"/>
+      <c r="AB41" s="23"/>
+      <c r="AC41" s="17"/>
       <c r="AD41" s="5"/>
       <c r="AE41" s="5"/>
-      <c r="AF41" s="27"/>
-      <c r="AG41" s="27"/>
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="10"/>
       <c r="AH41" s="5"/>
       <c r="AI41" s="5"/>
-      <c r="AJ41" s="33"/>
-      <c r="AK41" s="41"/>
-      <c r="AL41" s="41"/>
-      <c r="AM41" s="41"/>
-      <c r="AN41" s="34"/>
+      <c r="AJ41" s="16"/>
+      <c r="AK41" s="24"/>
+      <c r="AL41" s="24"/>
+      <c r="AM41" s="24"/>
+      <c r="AN41" s="17"/>
       <c r="AO41" s="6"/>
     </row>
     <row r="42" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2440,11 +2440,11 @@
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
       <c r="N42" s="5"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
@@ -2453,24 +2453,24 @@
       <c r="S42" s="5"/>
       <c r="T42" s="6"/>
       <c r="V42" s="4"/>
-      <c r="W42" s="33"/>
+      <c r="W42" s="16"/>
       <c r="X42" s="5"/>
       <c r="Y42" s="5"/>
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
       <c r="AB42" s="5"/>
-      <c r="AC42" s="34"/>
+      <c r="AC42" s="17"/>
       <c r="AD42" s="5"/>
       <c r="AE42" s="5"/>
       <c r="AF42" s="5"/>
       <c r="AG42" s="5"/>
       <c r="AH42" s="5"/>
       <c r="AI42" s="5"/>
-      <c r="AJ42" s="35"/>
-      <c r="AK42" s="36"/>
-      <c r="AL42" s="36"/>
-      <c r="AM42" s="36"/>
-      <c r="AN42" s="37"/>
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="19"/>
+      <c r="AL42" s="19"/>
+      <c r="AM42" s="19"/>
+      <c r="AN42" s="20"/>
       <c r="AO42" s="6"/>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.3">
@@ -2491,13 +2491,13 @@
       <c r="S43" s="5"/>
       <c r="T43" s="6"/>
       <c r="V43" s="4"/>
-      <c r="W43" s="35"/>
-      <c r="X43" s="36"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="36"/>
-      <c r="AA43" s="36"/>
-      <c r="AB43" s="36"/>
-      <c r="AC43" s="37"/>
+      <c r="W43" s="18"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="20"/>
       <c r="AD43" s="5"/>
       <c r="AE43" s="5"/>
       <c r="AF43" s="5"/>

</xml_diff>